<commit_message>
perbaikan css dan datatables
</commit_message>
<xml_diff>
--- a/public/dokumen/siswa2.xlsx
+++ b/public/dokumen/siswa2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kelulusan\public\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7405727-24ED-43E9-806D-61BC6D90545E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840AEC80-2F21-4338-B57A-77D9CDAD38C9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8550" xr2:uid="{882D24BE-8DA9-49AD-9D02-EC0A58D07275}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="1294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="1295">
   <si>
     <t>nama</t>
   </si>
@@ -3907,6 +3907,9 @@
   </si>
   <si>
     <t>LULUS</t>
+  </si>
+  <si>
+    <t>TIDAK LULUS</t>
   </si>
 </sst>
 </file>
@@ -4262,8 +4265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D54E1B-3F3F-4C20-B25F-02E86DA5C13D}">
   <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="J306" sqref="J306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13152,7 +13155,7 @@
         <v>67</v>
       </c>
       <c r="J306" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>